<commit_message>
update tables and suttas
</commit_message>
<xml_diff>
--- a/declensions & conjugations.xlsx
+++ b/declensions & conjugations.xlsx
@@ -3548,12 +3548,12 @@
     <t xml:space="preserve">atīsu</t>
   </si>
   <si>
+    <t xml:space="preserve">usu
+ūsu</t>
+  </si>
+  <si>
     <t xml:space="preserve">uyā
 uyaṃ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">usu
-ūsu</t>
   </si>
   <si>
     <t xml:space="preserve">kamme
@@ -39098,8 +39098,8 @@
   </sheetPr>
   <dimension ref="A1:DK350"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="CO1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="CT7" activeCellId="0" sqref="CT7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AX41" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BH44" activeCellId="0" sqref="BH44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -48007,7 +48007,7 @@
         <v>589</v>
       </c>
       <c r="BH43" s="40" t="s">
-        <v>817</v>
+        <v>1054</v>
       </c>
       <c r="BI43" s="54" t="s">
         <v>591</v>
@@ -48025,13 +48025,13 @@
         <v>587</v>
       </c>
       <c r="BR43" s="26" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="BS43" s="41" t="s">
         <v>593</v>
       </c>
       <c r="BT43" s="26" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="BU43" s="41" t="s">
         <v>595</v>
@@ -52416,7 +52416,7 @@
         <v>593</v>
       </c>
       <c r="H65" s="36" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="I65" s="48" t="s">
         <v>595</v>
@@ -54586,13 +54586,13 @@
         <v>587</v>
       </c>
       <c r="BR76" s="26" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="BS76" s="41" t="s">
         <v>593</v>
       </c>
       <c r="BT76" s="26" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="BU76" s="41" t="s">
         <v>595</v>

</xml_diff>

<commit_message>
x-word from front and back
</commit_message>
<xml_diff>
--- a/declensions & conjugations.xlsx
+++ b/declensions & conjugations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" state="visible" r:id="rId2"/>
@@ -2601,7 +2601,8 @@
   <si>
     <t xml:space="preserve">ini
 ismiṃ
-imhi</t>
+imhi
+ine</t>
   </si>
   <si>
     <t xml:space="preserve">isu
@@ -9431,7 +9432,7 @@
   </sheetPr>
   <dimension ref="A1:Z1024"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A113" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A113" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B127" activeCellId="0" sqref="B127"/>
     </sheetView>
   </sheetViews>
@@ -39127,8 +39128,8 @@
   </sheetPr>
   <dimension ref="A1:DK350"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="DA37" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="DC39" activeCellId="0" sqref="DC39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>